<commit_message>
[CODE] Firesight vision circle deconstructor
</commit_message>
<xml_diff>
--- a/Data/scar/ScarDoc_TFE.xlsx
+++ b/Data/scar/ScarDoc_TFE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Data\scar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608997F2-26DC-4E60-BCDA-4758EFA16B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A7B14-E803-40C6-A6DE-471853DDAE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="58">
   <si>
     <t>Class Name</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>EntityManager</t>
+  </si>
+  <si>
+    <t>Self</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,23 +582,23 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>49</v>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,7 +895,7 @@
         <v>53</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
[CODE] Initial setup for Resource Group deconstructors and notes making on it
</commit_message>
<xml_diff>
--- a/Data/scar/ScarDoc_TFE.xlsx
+++ b/Data/scar/ScarDoc_TFE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Data\scar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8A7B14-E803-40C6-A6DE-471853DDAE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A636C-AEC5-43DE-B4AC-52B71F6F1295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="62">
   <si>
     <t>Class Name</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>Self</t>
+  </si>
+  <si>
+    <t>Self Limiting</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Has deconstructor but needs to be implemented… This will be an ass to implement tbh….</t>
+  </si>
+  <si>
+    <t>Zombie Horde</t>
   </si>
 </sst>
 </file>
@@ -222,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +259,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,11 +284,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,11 +583,12 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -580,8 +607,11 @@
       <c r="F1" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -595,13 +625,14 @@
         <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -620,8 +651,9 @@
       <c r="F3" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -640,8 +672,9 @@
       <c r="F4" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -660,8 +693,9 @@
       <c r="F5" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -680,8 +714,9 @@
       <c r="F6" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -700,8 +735,9 @@
       <c r="F7" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -720,8 +756,9 @@
       <c r="F8" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -740,8 +777,9 @@
       <c r="F9" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -760,28 +798,32 @@
       <c r="F10" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -800,8 +842,9 @@
       <c r="F12" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -820,8 +863,9 @@
       <c r="F13" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -840,28 +884,30 @@
       <c r="F14" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -880,28 +926,30 @@
       <c r="F16" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -920,8 +968,9 @@
       <c r="F18" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -940,8 +989,9 @@
       <c r="F19" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -960,8 +1010,9 @@
       <c r="F20" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -980,8 +1031,9 @@
       <c r="F21" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1000,8 +1052,9 @@
       <c r="F22" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1020,8 +1073,9 @@
       <c r="F23" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1040,8 +1094,9 @@
       <c r="F24" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1060,28 +1115,30 @@
       <c r="F25" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1100,8 +1157,9 @@
       <c r="F27" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1120,8 +1178,9 @@
       <c r="F28" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1140,8 +1199,9 @@
       <c r="F29" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1160,8 +1220,9 @@
       <c r="F30" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1180,8 +1241,9 @@
       <c r="F31" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1200,26 +1262,28 @@
       <c r="F32" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="G33" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CODE] Improved deconstructors & Idle behaviour self limiting
</commit_message>
<xml_diff>
--- a/Data/scar/ScarDoc_TFE.xlsx
+++ b/Data/scar/ScarDoc_TFE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Data\scar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A636C-AEC5-43DE-B4AC-52B71F6F1295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6715049D-D596-4D89-AF56-78E5AD58BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,109 +1013,109 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="1"/>
+      <c r="D21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="D22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="1"/>
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="1"/>
+      <c r="D24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="1"/>
+      <c r="D25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">

</xml_diff>

<commit_message>
[CODE] Resource groups self limiting & minor refactor of attach leaders
Deatachable leaders now do not work with time travel so that will need to be adjusted later
</commit_message>
<xml_diff>
--- a/Data/scar/ScarDoc_TFE.xlsx
+++ b/Data/scar/ScarDoc_TFE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Data\scar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6715049D-D596-4D89-AF56-78E5AD58BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46686BF-BB97-4524-BD9F-F581EEDB103F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="61">
   <si>
     <t>Class Name</t>
   </si>
@@ -207,10 +207,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Has deconstructor but needs to be implemented… This will be an ass to implement tbh….</t>
-  </si>
-  <si>
-    <t>Zombie Horde</t>
+    <t>This is either self limiting or zombie, defined by programmer. Will default to self limiting which will destroy after 1 tick. Must explicitly be set to zombie</t>
   </si>
 </sst>
 </file>
@@ -234,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,12 +262,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,13 +275,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,40 +578,41 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="87.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="87.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -633,190 +638,190 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="1"/>
+      <c r="D3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="1"/>
+      <c r="D4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="1"/>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="1"/>
+      <c r="D6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="1"/>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="1"/>
+      <c r="D9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="D10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -824,193 +829,193 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="1"/>
+      <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="1"/>
+      <c r="D13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="1"/>
+      <c r="D14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="1"/>
+      <c r="D16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="1"/>
+      <c r="D18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="1"/>
+      <c r="D19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="1"/>
+      <c r="D20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1118,172 +1123,172 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="1"/>
+      <c r="D27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="1"/>
+      <c r="D28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="1"/>
+      <c r="D29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="1"/>
+      <c r="D30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="1"/>
+      <c r="D31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="1"/>
+      <c r="D32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>